<commit_message>
Sending lb3 table 1
</commit_message>
<xml_diff>
--- a/LR3/table_1_33.xlsx
+++ b/LR3/table_1_33.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prosk\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IT\IT_LR\LR3\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11112" windowHeight="8088"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -492,7 +492,7 @@
   </sheetPr>
   <dimension ref="A1:K1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>